<commit_message>
Some fixing and testing
</commit_message>
<xml_diff>
--- a/network_rates_10_0_0_5_eth0.xlsx
+++ b/network_rates_10_0_0_5_eth0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,8 +434,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
-    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -464,14 +464,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-02-23 18:00:12</t>
+          <t>2025-03-07 08:00:12</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.08068971633911133</v>
+        <v>0.0004563331604003906</v>
       </c>
       <c r="C2" t="n">
-        <v>5.164394569396973</v>
+        <v>0.001843929290771484</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
@@ -480,14 +480,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-02-23 18:00:22</t>
+          <t>2025-03-07 08:00:22</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05306072235107422</v>
+        <v>0.0007788658142089844</v>
       </c>
       <c r="C3" t="n">
-        <v>4.950971889495849</v>
+        <v>0.002700710296630859</v>
       </c>
       <c r="D3" t="n">
         <v>10</v>
@@ -496,14 +496,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-02-23 18:00:32</t>
+          <t>2025-03-07 08:00:32</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.07672691345214844</v>
+        <v>0.001163387298583984</v>
       </c>
       <c r="C4" t="n">
-        <v>5.755984783172607</v>
+        <v>0.00255422592163086</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
@@ -512,14 +512,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-02-23 18:00:42</t>
+          <t>2025-03-07 08:00:42</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01571083068847656</v>
+        <v>0.0005708694458007813</v>
       </c>
       <c r="C5" t="n">
-        <v>2.744588661193847</v>
+        <v>0.003145122528076172</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
@@ -528,14 +528,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-02-23 18:00:52</t>
+          <t>2025-03-07 08:00:52</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0460209846496582</v>
+        <v>0.0008191108703613281</v>
       </c>
       <c r="C6" t="n">
-        <v>4.038461303710937</v>
+        <v>0.002481460571289062</v>
       </c>
       <c r="D6" t="n">
         <v>10</v>
@@ -544,46 +544,46 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-02-23 18:01:02</t>
+          <t>2025-03-07 08:01:02</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08125953674316407</v>
+        <v>0.0004311130471425514</v>
       </c>
       <c r="C7" t="n">
-        <v>5.244959354400635</v>
+        <v>0.001758304241597325</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>10.001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-02-23 18:01:12</t>
+          <t>2025-03-07 08:01:12</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08229732513427734</v>
+        <v>0.0007921057303484254</v>
       </c>
       <c r="C8" t="n">
-        <v>6.182673549652099</v>
+        <v>0.002547423474036857</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>9.999000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-02-23 18:01:22</t>
+          <t>2025-03-07 08:01:22</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.04495353698730468</v>
+        <v>0.0007851600646972656</v>
       </c>
       <c r="C9" t="n">
-        <v>4.430321216583252</v>
+        <v>0.002597618103027344</v>
       </c>
       <c r="D9" t="n">
         <v>10</v>
@@ -592,46 +592,46 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-02-23 18:01:32</t>
+          <t>2025-03-07 08:01:32</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.07332855764446605</v>
+        <v>0.0009038925170898437</v>
       </c>
       <c r="C10" t="n">
-        <v>5.55556415677571</v>
+        <v>0.002462387084960938</v>
       </c>
       <c r="D10" t="n">
-        <v>10.006</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-02-23 18:01:42</t>
+          <t>2025-03-07 08:01:42</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.07983639594767603</v>
+        <v>0.0007788658142089844</v>
       </c>
       <c r="C11" t="n">
-        <v>5.988743965068005</v>
+        <v>0.002329826354980469</v>
       </c>
       <c r="D11" t="n">
-        <v>9.994</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-02-23 18:01:52</t>
+          <t>2025-03-07 08:01:52</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.05540904039478865</v>
+        <v>0.0008258947359658566</v>
       </c>
       <c r="C12" t="n">
-        <v>5.183512753766127</v>
+        <v>0.00236859477504398</v>
       </c>
       <c r="D12" t="n">
         <v>10.001</v>
@@ -640,14 +640,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-02-23 18:02:02</t>
+          <t>2025-03-07 08:02:02</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.07565911620458921</v>
+        <v>0.0004437890383276609</v>
       </c>
       <c r="C13" t="n">
-        <v>5.821357835399018</v>
+        <v>0.001871105384464228</v>
       </c>
       <c r="D13" t="n">
         <v>9.999000000000001</v>
@@ -656,14 +656,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-02-23 18:02:12</t>
+          <t>2025-03-07 08:02:12</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.06426334381103516</v>
+        <v>0.0007459640502929688</v>
       </c>
       <c r="C14" t="n">
-        <v>5.212989807128906</v>
+        <v>0.00227813720703125</v>
       </c>
       <c r="D14" t="n">
         <v>10</v>
@@ -672,14 +672,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-02-23 18:02:22</t>
+          <t>2025-03-07 08:02:22</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.04970455169677734</v>
+        <v>0.0007586479187011719</v>
       </c>
       <c r="C15" t="n">
-        <v>5.026263904571533</v>
+        <v>0.001813220977783203</v>
       </c>
       <c r="D15" t="n">
         <v>10</v>
@@ -688,14 +688,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-02-23 18:02:32</t>
+          <t>2025-03-07 08:02:32</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.03887805938720703</v>
+        <v>0.0009164810180664062</v>
       </c>
       <c r="C16" t="n">
-        <v>3.873053169250488</v>
+        <v>0.002518749237060547</v>
       </c>
       <c r="D16" t="n">
         <v>10</v>
@@ -704,14 +704,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-02-23 18:02:42</t>
+          <t>2025-03-07 08:02:42</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.06184225082397461</v>
+        <v>0.0007719993591308594</v>
       </c>
       <c r="C17" t="n">
-        <v>4.302584743499756</v>
+        <v>0.001801872253417969</v>
       </c>
       <c r="D17" t="n">
         <v>10</v>
@@ -720,14 +720,14 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-02-23 18:02:52</t>
+          <t>2025-03-07 08:02:52</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1032082557678223</v>
+        <v>0.0008254051208496094</v>
       </c>
       <c r="C18" t="n">
-        <v>6.465168285369873</v>
+        <v>0.003353595733642578</v>
       </c>
       <c r="D18" t="n">
         <v>10</v>
@@ -736,14 +736,14 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-02-23 18:03:02</t>
+          <t>2025-03-07 08:03:02</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.08187417984008789</v>
+        <v>0.0004569053649902344</v>
       </c>
       <c r="C19" t="n">
-        <v>5.341867351531983</v>
+        <v>0.001945018768310547</v>
       </c>
       <c r="D19" t="n">
         <v>10</v>
@@ -752,14 +752,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-02-23 18:03:12</t>
+          <t>2025-03-07 08:03:12</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.05695505142211914</v>
+        <v>0.0007857322692871094</v>
       </c>
       <c r="C20" t="n">
-        <v>4.587152290344238</v>
+        <v>0.002269840240478516</v>
       </c>
       <c r="D20" t="n">
         <v>10</v>
@@ -768,14 +768,14 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-02-23 18:03:22</t>
+          <t>2025-03-07 08:03:22</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.06972236633300781</v>
+        <v>0.0007914543151855469</v>
       </c>
       <c r="C21" t="n">
-        <v>4.490956211090088</v>
+        <v>0.002302837371826172</v>
       </c>
       <c r="D21" t="n">
         <v>10</v>
@@ -784,14 +784,14 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-02-23 18:03:32</t>
+          <t>2025-03-07 08:03:32</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.0833089828491211</v>
+        <v>0.000923919677734375</v>
       </c>
       <c r="C22" t="n">
-        <v>6.438681602478027</v>
+        <v>0.002357769012451172</v>
       </c>
       <c r="D22" t="n">
         <v>10</v>
@@ -800,14 +800,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-02-23 18:03:42</t>
+          <t>2025-03-07 08:03:42</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.08310508728027344</v>
+        <v>0.0008040428161621094</v>
       </c>
       <c r="C23" t="n">
-        <v>5.112808227539062</v>
+        <v>0.003762626647949219</v>
       </c>
       <c r="D23" t="n">
         <v>10</v>
@@ -816,62 +816,62 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-02-23 18:03:52</t>
+          <t>2025-03-07 08:03:52</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.07054233551025391</v>
+        <v>0.0008121631989633068</v>
       </c>
       <c r="C24" t="n">
-        <v>5.194169807434082</v>
+        <v>0.001633003966449058</v>
       </c>
       <c r="D24" t="n">
-        <v>10</v>
+        <v>10.001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-02-23 18:04:02</t>
+          <t>2025-03-07 08:04:02</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.07158088131006236</v>
+        <v>0.0004437890383276609</v>
       </c>
       <c r="C25" t="n">
-        <v>4.907438104456157</v>
+        <v>0.001865859651150662</v>
       </c>
       <c r="D25" t="n">
-        <v>10.001</v>
+        <v>9.999000000000001</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-02-23 18:04:12</t>
+          <t>2025-03-07 08:04:12</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.07784439332605135</v>
+        <v>0.0007920265197753906</v>
       </c>
       <c r="C26" t="n">
-        <v>5.018909808003505</v>
+        <v>0.002366065979003906</v>
       </c>
       <c r="D26" t="n">
-        <v>9.999000000000001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-02-23 18:04:22</t>
+          <t>2025-03-07 08:04:22</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.07523670196533203</v>
+        <v>0.0007857322692871094</v>
       </c>
       <c r="C27" t="n">
-        <v>4.548470497131348</v>
+        <v>0.002358055114746094</v>
       </c>
       <c r="D27" t="n">
         <v>10</v>
@@ -880,14 +880,14 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-02-23 18:04:32</t>
+          <t>2025-03-07 08:04:32</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.03380393981933594</v>
+        <v>0.0008913040161132813</v>
       </c>
       <c r="C28" t="n">
-        <v>4.543086147308349</v>
+        <v>0.002303218841552734</v>
       </c>
       <c r="D28" t="n">
         <v>10</v>
@@ -896,14 +896,14 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-02-23 18:04:42</t>
+          <t>2025-03-07 08:04:42</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.05266828536987304</v>
+        <v>0.0007983207702636719</v>
       </c>
       <c r="C29" t="n">
-        <v>4.202507591247558</v>
+        <v>0.003310489654541016</v>
       </c>
       <c r="D29" t="n">
         <v>10</v>
@@ -912,46 +912,46 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-02-23 18:04:52</t>
+          <t>2025-03-07 08:04:52</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.04519501647034606</v>
+        <v>0.0008379936218261719</v>
       </c>
       <c r="C30" t="n">
-        <v>4.025069721690663</v>
+        <v>0.002953720092773437</v>
       </c>
       <c r="D30" t="n">
-        <v>10.01</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-02-23 18:05:02</t>
+          <t>2025-03-07 08:05:02</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.08724048450305774</v>
+        <v>0.0004111289978027344</v>
       </c>
       <c r="C31" t="n">
-        <v>5.545258164047837</v>
+        <v>0.001021766662597656</v>
       </c>
       <c r="D31" t="n">
-        <v>9.99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-02-23 18:05:12</t>
+          <t>2025-03-07 08:05:12</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.02928285598754883</v>
+        <v>0.0007788658142089844</v>
       </c>
       <c r="C32" t="n">
-        <v>3.736904239654541</v>
+        <v>0.001802539825439453</v>
       </c>
       <c r="D32" t="n">
         <v>10</v>
@@ -960,46 +960,46 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-02-23 18:05:22</t>
+          <t>2025-03-07 08:05:22</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.06485319137573242</v>
+        <v>0.0007913751776677801</v>
       </c>
       <c r="C33" t="n">
-        <v>5.146582221984863</v>
+        <v>0.002338080248371647</v>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
+        <v>10.001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-02-23 18:05:32</t>
+          <t>2025-03-07 08:05:32</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.04726533889770508</v>
+        <v>0.0009102777953576607</v>
       </c>
       <c r="C34" t="n">
-        <v>3.703241729736328</v>
+        <v>0.002016555262704005</v>
       </c>
       <c r="D34" t="n">
-        <v>10</v>
+        <v>9.999000000000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-02-23 18:05:42</t>
+          <t>2025-03-07 08:05:42</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.03320951461791992</v>
+        <v>0.0008109092712402343</v>
       </c>
       <c r="C35" t="n">
-        <v>3.237907600402832</v>
+        <v>0.003480720520019531</v>
       </c>
       <c r="D35" t="n">
         <v>10</v>
@@ -1008,14 +1008,14 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-02-23 18:05:52</t>
+          <t>2025-03-07 08:05:52</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.05819453989049338</v>
+        <v>0.0008253225885907503</v>
       </c>
       <c r="C36" t="n">
-        <v>4.548205743848223</v>
+        <v>0.002395294985882271</v>
       </c>
       <c r="D36" t="n">
         <v>10.001</v>
@@ -1024,46 +1024,46 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-02-23 18:06:02</t>
+          <t>2025-03-07 08:06:02</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.05437078475952149</v>
+        <v>0.0004437890383276609</v>
       </c>
       <c r="C37" t="n">
-        <v>3.955227851867676</v>
+        <v>0.001911163711586002</v>
       </c>
       <c r="D37" t="n">
-        <v>10</v>
+        <v>9.999000000000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-02-23 18:06:12</t>
+          <t>2025-03-07 08:06:12</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.08420947075176267</v>
+        <v>0.0007983207702636719</v>
       </c>
       <c r="C38" t="n">
-        <v>5.425523097353681</v>
+        <v>0.002164649963378906</v>
       </c>
       <c r="D38" t="n">
-        <v>9.999000000000001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-02-23 18:06:22</t>
+          <t>2025-03-07 08:06:22</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.02524623870849609</v>
+        <v>0.0007857322692871094</v>
       </c>
       <c r="C39" t="n">
-        <v>3.610650157928467</v>
+        <v>0.00225677490234375</v>
       </c>
       <c r="D39" t="n">
         <v>10</v>
@@ -1072,14 +1072,14 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-02-23 18:06:32</t>
+          <t>2025-03-07 08:06:32</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.04127779006958008</v>
+        <v>0.0009050369262695312</v>
       </c>
       <c r="C40" t="n">
-        <v>3.460038471221924</v>
+        <v>0.00279397964477539</v>
       </c>
       <c r="D40" t="n">
         <v>10</v>
@@ -1088,14 +1088,14 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-02-23 18:06:42</t>
+          <t>2025-03-07 08:06:42</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.06351919174194336</v>
+        <v>0.0007971763610839844</v>
       </c>
       <c r="C41" t="n">
-        <v>4.592228698730469</v>
+        <v>0.002548599243164063</v>
       </c>
       <c r="D41" t="n">
         <v>10</v>
@@ -1104,46 +1104,46 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-02-23 18:06:52</t>
+          <t>2025-03-07 08:06:52</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.03980705826512076</v>
+        <v>0.0008122444152832032</v>
       </c>
       <c r="C42" t="n">
-        <v>2.906274180473798</v>
+        <v>0.001927947998046875</v>
       </c>
       <c r="D42" t="n">
-        <v>10.001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-02-23 18:07:02</t>
+          <t>2025-03-07 08:07:02</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.05307671117453542</v>
+        <v>0.0004437446594238281</v>
       </c>
       <c r="C43" t="n">
-        <v>3.420930491028839</v>
+        <v>0.001998710632324219</v>
       </c>
       <c r="D43" t="n">
-        <v>9.999000000000001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-02-23 18:07:12</t>
+          <t>2025-03-07 08:07:12</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.03971996307373047</v>
+        <v>0.0007983207702636719</v>
       </c>
       <c r="C44" t="n">
-        <v>2.396373653411865</v>
+        <v>0.002361965179443359</v>
       </c>
       <c r="D44" t="n">
         <v>10</v>
@@ -1152,46 +1152,46 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-02-23 18:07:22</t>
+          <t>2025-03-07 08:07:22</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.01105422973632813</v>
+        <v>0.0009670244218253956</v>
       </c>
       <c r="C45" t="n">
-        <v>0.4582766532897949</v>
+        <v>0.003090454046636352</v>
       </c>
       <c r="D45" t="n">
-        <v>10</v>
+        <v>10.001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-02-23 18:07:32</t>
+          <t>2025-03-07 08:07:32</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.05145130157470703</v>
+        <v>0.0009108500571736861</v>
       </c>
       <c r="C46" t="n">
-        <v>3.730493259429932</v>
+        <v>0.0020096881209117</v>
       </c>
       <c r="D46" t="n">
-        <v>10</v>
+        <v>9.999000000000001</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-02-23 18:07:42</t>
+          <t>2025-03-07 08:07:42</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.07207241058349609</v>
+        <v>0.0008303642272949219</v>
       </c>
       <c r="C47" t="n">
-        <v>5.193370723724366</v>
+        <v>0.003392601013183594</v>
       </c>
       <c r="D47" t="n">
         <v>10</v>
@@ -1200,14 +1200,14 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-02-23 18:07:52</t>
+          <t>2025-03-07 08:07:52</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.07146196365356446</v>
+        <v>0.0008322715759277344</v>
       </c>
       <c r="C48" t="n">
-        <v>5.2863374710083</v>
+        <v>0.002427959442138672</v>
       </c>
       <c r="D48" t="n">
         <v>10</v>
@@ -1216,14 +1216,14 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-02-23 18:08:02</t>
+          <t>2025-03-07 08:08:02</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.07496213912963867</v>
+        <v>0.0004506111145019531</v>
       </c>
       <c r="C49" t="n">
-        <v>5.146772861480713</v>
+        <v>0.001979541778564453</v>
       </c>
       <c r="D49" t="n">
         <v>10</v>
@@ -1232,14 +1232,14 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-02-23 18:08:12</t>
+          <t>2025-03-07 08:08:12</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.06270151138305664</v>
+        <v>0.0007920265197753906</v>
       </c>
       <c r="C50" t="n">
-        <v>5.143784999847412</v>
+        <v>0.002208614349365234</v>
       </c>
       <c r="D50" t="n">
         <v>10</v>
@@ -1248,14 +1248,14 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-02-23 18:08:22</t>
+          <t>2025-03-07 08:08:22</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.05326471328735351</v>
+        <v>0.0004574775695800781</v>
       </c>
       <c r="C51" t="n">
-        <v>4.171600818634033</v>
+        <v>0.001810359954833984</v>
       </c>
       <c r="D51" t="n">
         <v>10</v>
@@ -1264,14 +1264,14 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-02-23 18:08:32</t>
+          <t>2025-03-07 08:08:32</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.03666396665997463</v>
+        <v>0.001257770646275216</v>
       </c>
       <c r="C52" t="n">
-        <v>3.541689707677182</v>
+        <v>0.002831938790984183</v>
       </c>
       <c r="D52" t="n">
         <v>10.001</v>
@@ -1280,14 +1280,14 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-02-23 18:08:42</t>
+          <t>2025-03-07 08:08:42</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.06441932187603526</v>
+        <v>0.0008104181084612367</v>
       </c>
       <c r="C53" t="n">
-        <v>5.210411979003076</v>
+        <v>0.0032669473307194</v>
       </c>
       <c r="D53" t="n">
         <v>9.999000000000001</v>
@@ -1296,46 +1296,46 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-02-23 18:08:52</t>
+          <t>2025-03-07 08:08:52</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.06194810867309571</v>
+        <v>0.0004908070899453024</v>
       </c>
       <c r="C54" t="n">
-        <v>4.736636829376221</v>
+        <v>0.002478542428960229</v>
       </c>
       <c r="D54" t="n">
-        <v>10</v>
+        <v>10.001</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-02-23 18:09:02</t>
+          <t>2025-03-07 08:09:02</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.07625665664672851</v>
+        <v>0.0007852385885561212</v>
       </c>
       <c r="C55" t="n">
-        <v>4.895595073699951</v>
+        <v>0.001499325957986424</v>
       </c>
       <c r="D55" t="n">
-        <v>10</v>
+        <v>9.999000000000001</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-02-23 18:09:12</t>
+          <t>2025-03-07 08:09:12</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.07829675674438477</v>
+        <v>0.0008002281188964844</v>
       </c>
       <c r="C56" t="n">
-        <v>5.28487663269043</v>
+        <v>0.002418804168701172</v>
       </c>
       <c r="D56" t="n">
         <v>10</v>
@@ -1344,46 +1344,46 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-02-23 18:09:22</t>
+          <t>2025-03-07 08:09:22</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.07503827253993352</v>
+        <v>0.0004443168640136719</v>
       </c>
       <c r="C57" t="n">
-        <v>6.11403360091237</v>
+        <v>0.001771068572998047</v>
       </c>
       <c r="D57" t="n">
-        <v>10.001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-02-23 18:09:32</t>
+          <t>2025-03-07 08:09:32</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.05808104537870779</v>
+        <v>0.001257896423339844</v>
       </c>
       <c r="C58" t="n">
-        <v>4.137379584973878</v>
+        <v>0.002708721160888672</v>
       </c>
       <c r="D58" t="n">
-        <v>9.999000000000001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-02-23 18:09:42</t>
+          <t>2025-03-07 08:09:42</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.0657423973083496</v>
+        <v>0.0008040428161621094</v>
       </c>
       <c r="C59" t="n">
-        <v>5.137449169158936</v>
+        <v>0.00345001220703125</v>
       </c>
       <c r="D59" t="n">
         <v>10</v>
@@ -1392,30 +1392,30 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-02-23 18:09:52</t>
+          <t>2025-03-07 08:09:52</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.04321346282958984</v>
+        <v>0.0004713540791916902</v>
       </c>
       <c r="C60" t="n">
-        <v>4.278071022033691</v>
+        <v>0.001810751084315397</v>
       </c>
       <c r="D60" t="n">
-        <v>10</v>
+        <v>10.001</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>AVERAGE</t>
+          <t>2025-03-07 08:10:02</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.0603828432430764</v>
+        <v>0.0008046150207519532</v>
       </c>
       <c r="C61" t="n">
-        <v>4.618726067751225</v>
+        <v>0.002696514129638672</v>
       </c>
       <c r="D61" t="n">
         <v>10</v>
@@ -1424,17 +1424,1729 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>2025-03-07 08:10:12</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.0007789437085798423</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.001537285991782772</v>
+      </c>
+      <c r="D62" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:10:22</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.0004437446594238281</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.001922988891601563</v>
+      </c>
+      <c r="D63" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:10:32</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.001252174377441406</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.002797222137451172</v>
+      </c>
+      <c r="D64" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:10:42</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.0007988929748535157</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.003263282775878906</v>
+      </c>
+      <c r="D65" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:10:52</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.0004971504211425781</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.001978015899658203</v>
+      </c>
+      <c r="D66" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:11:02</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.0007983207702636719</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.002478599548339844</v>
+      </c>
+      <c r="D67" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:11:12</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.0007788658142089844</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.002057647705078125</v>
+      </c>
+      <c r="D68" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:11:22</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.0004569053649902344</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.002312374114990234</v>
+      </c>
+      <c r="D69" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:11:32</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.00123888978289671</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.001891233148413674</v>
+      </c>
+      <c r="D70" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:11:42</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0008172852502535409</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.003322647480812534</v>
+      </c>
+      <c r="D71" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:11:52</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.0004908561706542969</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.002079296112060547</v>
+      </c>
+      <c r="D72" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:12:02</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.0007851600646972656</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.001885032653808594</v>
+      </c>
+      <c r="D73" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:12:12</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.0007983207702636719</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.002269268035888672</v>
+      </c>
+      <c r="D74" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:12:22</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.0004506111145019531</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.001848697662353516</v>
+      </c>
+      <c r="D75" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:12:32</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.001245307922363281</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.002598762512207031</v>
+      </c>
+      <c r="D76" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:12:42</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.0008172035217285156</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.003380584716796875</v>
+      </c>
+      <c r="D77" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:12:52</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0004714012145996094</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.001935482025146484</v>
+      </c>
+      <c r="D78" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:13:02</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.0008046150207519532</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.002719974517822266</v>
+      </c>
+      <c r="D79" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:13:12</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.0007782936096191406</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.001531600952148438</v>
+      </c>
+      <c r="D80" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:13:22</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.0004443168640136719</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.001899623870849609</v>
+      </c>
+      <c r="D81" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:13:32</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.001244735717773438</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.002158546447753906</v>
+      </c>
+      <c r="D82" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:13:42</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.0008045345672952237</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.003201450637406962</v>
+      </c>
+      <c r="D83" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:13:52</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.000484610381204136</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.001971060448329989</v>
+      </c>
+      <c r="D84" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:14:02</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0.0007983207702636719</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.002648735046386719</v>
+      </c>
+      <c r="D85" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:14:12</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0.0007914543151855469</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.002261066436767578</v>
+      </c>
+      <c r="D86" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:14:22</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0.0004569053649902344</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.001836299896240234</v>
+      </c>
+      <c r="D87" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:14:32</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0.001251602172851563</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.002642822265625</v>
+      </c>
+      <c r="D88" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:14:42</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.0008103370666503907</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.003338241577148438</v>
+      </c>
+      <c r="D89" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:14:52</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.0004782676696777344</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.001943874359130859</v>
+      </c>
+      <c r="D90" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:15:02</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.0007851600646972656</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.002311897277832031</v>
+      </c>
+      <c r="D91" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:15:12</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0.0007914543151855469</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.002744770050048828</v>
+      </c>
+      <c r="D92" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:15:22</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>0.0004242897033691406</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.0009720802307128906</v>
+      </c>
+      <c r="D93" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:15:32</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0.001251602172851563</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.002635955810546875</v>
+      </c>
+      <c r="D94" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:15:42</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.0007654190063476563</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.003376007080078125</v>
+      </c>
+      <c r="D95" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:15:52</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.0004832267761230469</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.001760292053222656</v>
+      </c>
+      <c r="D96" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:16:02</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0.0007857322692871094</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.002356910705566406</v>
+      </c>
+      <c r="D97" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:16:12</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0.0007914543151855469</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.002243232727050781</v>
+      </c>
+      <c r="D98" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:16:22</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0.0004442724367699949</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.001631859671698846</v>
+      </c>
+      <c r="D99" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:16:32</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0.001251727345586121</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.003030317069792916</v>
+      </c>
+      <c r="D100" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:16:42</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0.0008046150207519532</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.003058528900146484</v>
+      </c>
+      <c r="D101" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:16:52</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0.0004713540791916902</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.001879694843015699</v>
+      </c>
+      <c r="D102" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:17:02</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0.0007719993591308594</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.001592731475830078</v>
+      </c>
+      <c r="D103" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:17:12</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0.0006901477501265751</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0.00187568347899243</v>
+      </c>
+      <c r="D104" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:17:22</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0.0007396697998046875</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0.003050613403320313</v>
+      </c>
+      <c r="D105" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:17:32</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>0.0009107589721679688</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.002003765106201172</v>
+      </c>
+      <c r="D106" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:17:42</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>0.0008040428161621094</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.003427886962890625</v>
+      </c>
+      <c r="D107" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:17:52</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>0.0008322715759277344</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.002303600311279297</v>
+      </c>
+      <c r="D108" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:18:02</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>0.0004500389099121094</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.002243709564208984</v>
+      </c>
+      <c r="D109" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:18:12</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>0.0007719993591308594</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0.001574516296386719</v>
+      </c>
+      <c r="D110" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:18:22</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>0.0007914543151855469</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.002354621887207031</v>
+      </c>
+      <c r="D111" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:18:32</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>0.0009106679053774311</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.002124955351144573</v>
+      </c>
+      <c r="D112" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:18:42</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>0.0008104181084612367</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.003270285524646214</v>
+      </c>
+      <c r="D113" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:18:52</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>0.0008448600769042969</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.0024566650390625</v>
+      </c>
+      <c r="D114" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:19:02</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>0.0004499939105210573</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.002177116120175092</v>
+      </c>
+      <c r="D115" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:19:12</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>0.0007720765667875381</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.001535092321488008</v>
+      </c>
+      <c r="D116" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:19:22</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>0.0007914543151855469</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.002318382263183594</v>
+      </c>
+      <c r="D117" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:19:32</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>0.000910186767578125</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.003149509429931641</v>
+      </c>
+      <c r="D118" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:19:42</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>0.0007914543151855469</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0.002278804779052734</v>
+      </c>
+      <c r="D119" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:19:52</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>0.0008404731750488281</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.002271842956542969</v>
+      </c>
+      <c r="D120" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:20:02</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>0.0004443168640136719</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0.001881027221679688</v>
+      </c>
+      <c r="D121" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:20:12</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>0.0007719993591308594</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0.001782321929931641</v>
+      </c>
+      <c r="D122" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:20:22</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>0.0004311561584472656</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0.001653861999511719</v>
+      </c>
+      <c r="D123" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:20:32</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>0.001252174377441406</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0.0025604248046875</v>
+      </c>
+      <c r="D124" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:20:42</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>0.0008046150207519532</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0.00293893814086914</v>
+      </c>
+      <c r="D125" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:20:52</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>0.0004494667053222656</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0.00203542709350586</v>
+      </c>
+      <c r="D126" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:21:02</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>0.0008254051208496094</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0.002470493316650391</v>
+      </c>
+      <c r="D127" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:21:12</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>0.0007914543151855469</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0.002173900604248047</v>
+      </c>
+      <c r="D128" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:21:22</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>0.0004637718200683594</v>
+      </c>
+      <c r="C129" t="n">
+        <v>0.001858329772949219</v>
+      </c>
+      <c r="D129" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:21:32</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>0.001252174377441406</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0.002578449249267578</v>
+      </c>
+      <c r="D130" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:21:42</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>0.0008103370666503907</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.003337478637695312</v>
+      </c>
+      <c r="D131" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:21:52</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>0.0004374504089355469</v>
+      </c>
+      <c r="C132" t="n">
+        <v>0.002200508117675781</v>
+      </c>
+      <c r="D132" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:22:02</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>0.0008254051208496094</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0.001637077331542969</v>
+      </c>
+      <c r="D133" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:22:12</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>0.0007851600646972656</v>
+      </c>
+      <c r="C134" t="n">
+        <v>0.002186870574951172</v>
+      </c>
+      <c r="D134" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:22:22</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>0.0004506111145019531</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0.0018585205078125</v>
+      </c>
+      <c r="D135" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:22:32</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>0.001245755551397985</v>
+      </c>
+      <c r="C136" t="n">
+        <v>0.002663250673223693</v>
+      </c>
+      <c r="D136" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:22:42</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>0.0007978283485086789</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0.003410394292603088</v>
+      </c>
+      <c r="D137" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:22:52</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>0.0004374504089355469</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0.001761817932128906</v>
+      </c>
+      <c r="D138" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:23:02</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>0.0008316993713378906</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0.002766990661621094</v>
+      </c>
+      <c r="D139" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:23:12</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>0.0004305839538574219</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.0010040283203125</v>
+      </c>
+      <c r="D140" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:23:22</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>0.0007851600646972656</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.002296638488769531</v>
+      </c>
+      <c r="D141" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:23:32</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>0.001232147216796875</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0.001990032196044922</v>
+      </c>
+      <c r="D142" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:23:42</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>0.0004757881164550781</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0.003039360046386719</v>
+      </c>
+      <c r="D143" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:23:52</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>0.0007920265197753906</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0.002321052551269531</v>
+      </c>
+      <c r="D144" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:24:02</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>0.0008322715759277344</v>
+      </c>
+      <c r="C145" t="n">
+        <v>0.002204704284667969</v>
+      </c>
+      <c r="D145" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:24:12</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>0.0004443168640136719</v>
+      </c>
+      <c r="C146" t="n">
+        <v>0.001835536956787109</v>
+      </c>
+      <c r="D146" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:24:22</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>0.0008108281884213923</v>
+      </c>
+      <c r="C147" t="n">
+        <v>0.002762041453325371</v>
+      </c>
+      <c r="D147" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:24:32</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>0.001244860203793817</v>
+      </c>
+      <c r="C148" t="n">
+        <v>0.001939586048448595</v>
+      </c>
+      <c r="D148" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:24:42</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>0.0004913330078125</v>
+      </c>
+      <c r="C149" t="n">
+        <v>0.003133010864257812</v>
+      </c>
+      <c r="D149" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:24:52</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>0.0007920265197753906</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0.002250766754150391</v>
+      </c>
+      <c r="D150" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:25:02</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0.0008259773254394531</v>
+      </c>
+      <c r="C151" t="n">
+        <v>0.002431297302246094</v>
+      </c>
+      <c r="D151" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:25:12</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0.0004511833190917969</v>
+      </c>
+      <c r="C152" t="n">
+        <v>0.001744174957275391</v>
+      </c>
+      <c r="D152" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:25:22</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>0.0007977485656738281</v>
+      </c>
+      <c r="C153" t="n">
+        <v>0.002623558044433594</v>
+      </c>
+      <c r="D153" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:25:32</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0.001257896423339844</v>
+      </c>
+      <c r="C154" t="n">
+        <v>0.002858543395996094</v>
+      </c>
+      <c r="D154" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:25:42</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>0.0004374504089355469</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0.001806259155273438</v>
+      </c>
+      <c r="D155" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:25:52</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0.0007980015696358176</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0.00227751230440441</v>
+      </c>
+      <c r="D156" t="n">
+        <v>10.004</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:26:02</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0.0008388174716575129</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0.002460645725455918</v>
+      </c>
+      <c r="D157" t="n">
+        <v>9.997</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:26:12</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0.0004449335619597116</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0.001728516815304577</v>
+      </c>
+      <c r="D158" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:26:22</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0.0007920265197753906</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0.002157974243164063</v>
+      </c>
+      <c r="D159" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:26:32</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>0.001252174377441406</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0.002671146392822266</v>
+      </c>
+      <c r="D160" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:26:42</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0.0004574775695800781</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0.003074359893798828</v>
+      </c>
+      <c r="D161" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:26:52</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0.0007983207702636719</v>
+      </c>
+      <c r="C162" t="n">
+        <v>0.002439308166503906</v>
+      </c>
+      <c r="D162" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:27:02</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0.0008121631989633068</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0.001624612471614167</v>
+      </c>
+      <c r="D163" t="n">
+        <v>10.001</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:27:12</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0.000437494158351382</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0.001650307700447779</v>
+      </c>
+      <c r="D164" t="n">
+        <v>9.999000000000001</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:27:22</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0.001029491424560547</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0.00327606201171875</v>
+      </c>
+      <c r="D165" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:27:32</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0.001264190673828125</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0.00352783203125</v>
+      </c>
+      <c r="D166" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2025-03-07 08:27:42</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>0.0004437446594238281</v>
+      </c>
+      <c r="C167" t="n">
+        <v>0.001837921142578125</v>
+      </c>
+      <c r="D167" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>AVERAGE</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0.0007587457572869635</v>
+      </c>
+      <c r="C168" t="n">
+        <v>0.00234440542912657</v>
+      </c>
+      <c r="D168" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
           <t>MAX</t>
         </is>
       </c>
-      <c r="B62" t="n">
-        <v>0.1032082557678223</v>
-      </c>
-      <c r="C62" t="n">
-        <v>6.465168285369873</v>
-      </c>
-      <c r="D62" t="n">
-        <v>10.01</v>
+      <c r="B169" t="n">
+        <v>0.001264190673828125</v>
+      </c>
+      <c r="C169" t="n">
+        <v>0.003762626647949219</v>
+      </c>
+      <c r="D169" t="n">
+        <v>10.004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>